<commit_message>
Updated sheet and Sequence for user readability and ordering exceptions
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005F9C89-3EBA-4523-8A31-CFC40CB18C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0043DC4B-E1F3-4F38-A134-EB540B6E96AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1668" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
+    <workbookView xWindow="0" yWindow="2712" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Customer 2" sheetId="3" r:id="rId3"/>
     <sheet name="Customer 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Customers</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Quantity Ordered</t>
   </si>
   <si>
     <t>bestPrices</t>
@@ -155,39 +158,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table8" displayName="Table8" ref="A1:E6" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table8" displayName="Table8" ref="A1:F6" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table9" displayName="Table9" ref="A1:E6" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table9" displayName="Table9" ref="A1:F6" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table10" displayName="Table10" ref="A1:E6" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table10" displayName="Table10" ref="A1:F6" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -493,7 +499,7 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2 A2 A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,19 +581,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DE327F-B7D9-4E04-AF5A-56B7991B2F90}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -603,62 +611,61 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4">
-        <f>VALUE(D2)*Table8[[#This Row],[Column2]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <f>VALUE(E2)*Table8[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <f>VALUE(E3)*Table8[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4">
-        <f>VALUE(D3)*Table8[[#This Row],[Column2]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="F4" s="4">
+        <f>VALUE(E4)*Table8[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
-        <f>VALUE(D4)*Table8[[#This Row],[Column2]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4">
-        <f>VALUE(D5)*Table8[[#This Row],[Column2]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
-        <f>SUM(E2:E5)</f>
+      <c r="F5" s="4">
+        <f>VALUE(E5)*Table8[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
     </row>
@@ -673,20 +680,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AFAD3A-2B7D-4C7F-B9F6-559E4CC27AFE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="D2" sqref="D2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -702,61 +711,61 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="4">
-        <f>SUM(E2:E5)</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
     </row>
@@ -770,15 +779,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EE7A7E-2160-4409-A677-51D38C07218F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -794,66 +811,61 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4">
+        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4">
-        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2"/>
       <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4">
-        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>16</v>
+      </c>
       <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4">
-        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>11</v>
+      </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4">
-        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column5]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="4">
-        <f>SUM(E2:E5)</f>
+      <c r="F5" s="4">
+        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added quantity wanted feature to add customer and ability to see how much of each item is wanted on shopping list in Customer sequence
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0043DC4B-E1F3-4F38-A134-EB540B6E96AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66DA34-47E8-4431-B90D-0828E9032950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2712" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
+    <workbookView xWindow="3576" yWindow="2124" windowWidth="17280" windowHeight="8964" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,14 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,74 +495,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897428BC-5AFF-4372-82AD-8C60F06E5890}">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2 A2:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="9.109375" style="2" customWidth="1"/>
-    <col min="5" max="7" width="10.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="2" customWidth="1"/>
-    <col min="9" max="11" width="10.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="2" customWidth="1"/>
-    <col min="13" max="15" width="10.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="2" customWidth="1"/>
-    <col min="17" max="20" width="10.109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.109375" style="2" customWidth="1"/>
-    <col min="22" max="25" width="10.109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.109375" style="2" customWidth="1"/>
-    <col min="27" max="30" width="10.109375" style="2" customWidth="1"/>
+    <col min="1" max="4" width="9.109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="10.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="11" width="10.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
+    <col min="13" max="15" width="10.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="20" width="10.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" style="1" customWidth="1"/>
+    <col min="22" max="25" width="10.109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" style="1" customWidth="1"/>
+    <col min="27" max="30" width="10.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="G6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -584,87 +577,87 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="4" width="17.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="17.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f>VALUE(E2)*Table8[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>VALUE(E3)*Table8[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f>VALUE(E4)*Table8[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <f>VALUE(E5)*Table8[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
@@ -688,83 +681,83 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>
@@ -781,90 +774,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EE7A7E-2160-4409-A677-51D38C07218F}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f>SUM(F2:F5)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
"Updates prior to swiching to main on 10/14/2021"
</commit_message>
<xml_diff>
--- a/Customers.xlsx
+++ b/Customers.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66DA34-47E8-4431-B90D-0828E9032950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14BF7B-23C3-41FA-9064-C5E245E19297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="2124" windowWidth="17280" windowHeight="8964" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
+    <workbookView xWindow="9240" yWindow="2568" windowWidth="10968" windowHeight="8964" xr2:uid="{614A50CF-43C8-4490-B4B7-34731EEDD18F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Customer 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Customer 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Customer 4" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Customer 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Customer 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Customer 3" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Customers</t>
   </si>
@@ -72,22 +73,85 @@
     <t>Milk</t>
   </si>
   <si>
+    <t>Milk Sold Out</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>0.5496</t>
+  </si>
+  <si>
     <t>Soap</t>
   </si>
   <si>
+    <t>Soap Sold Out</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.5489</t>
+  </si>
+  <si>
     <t>Bananas</t>
   </si>
   <si>
+    <t>Bananas Sold Out</t>
+  </si>
+  <si>
     <t>Hennessy</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>104.99</t>
+  </si>
+  <si>
     <t>Toothpaste</t>
   </si>
   <si>
+    <t>Toothpaste Sold Out</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
     <t>Cake</t>
   </si>
   <si>
+    <t>68</t>
+  </si>
+  <si>
     <t>Cookies</t>
+  </si>
+  <si>
+    <t>Cookies Sold Out</t>
+  </si>
+  <si>
+    <t>2.055</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Customer 4</t>
+  </si>
+  <si>
+    <t>bestPrice</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>apples</t>
   </si>
 </sst>
 </file>
@@ -134,11 +198,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,68 +558,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4939FD86-26EB-431A-B239-6EE8666F5D36}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897428BC-5AFF-4372-82AD-8C60F06E5890}">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8 F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="9.109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="10.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
-    <col min="9" max="11" width="10.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
-    <col min="13" max="15" width="10.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
-    <col min="17" max="20" width="10.109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.109375" style="1" customWidth="1"/>
-    <col min="22" max="25" width="10.109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.109375" style="1" customWidth="1"/>
-    <col min="27" max="30" width="10.109375" style="1" customWidth="1"/>
+    <col min="1" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="10.109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="2" customWidth="1"/>
+    <col min="13" max="15" width="10.109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="2" customWidth="1"/>
+    <col min="17" max="20" width="10.109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" style="2" customWidth="1"/>
+    <col min="22" max="25" width="10.109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" style="2" customWidth="1"/>
+    <col min="27" max="30" width="10.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -572,94 +703,124 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DE327F-B7D9-4E04-AF5A-56B7991B2F90}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2 D2 D2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="17.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="4" width="17.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
         <v>6</v>
       </c>
-      <c r="F2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3">
         <f>VALUE(E2)*Table8[[#This Row],[Column6]]</f>
-        <v>0</v>
+        <v>2.1983999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3">
         <f>VALUE(E3)*Table8[[#This Row],[Column6]]</f>
-        <v>0</v>
+        <v>0.54890000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <f>VALUE(E4)*Table8[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3">
         <f>VALUE(E5)*Table8[[#This Row],[Column6]]</f>
-        <v>0</v>
+        <v>314.96999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f>SUM(F2:F5)</f>
-        <v>0</v>
+        <v>317.71729999999997</v>
       </c>
     </row>
   </sheetData>
@@ -671,95 +832,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AFAD3A-2B7D-4C7F-B9F6-559E4CC27AFE}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E10"/>
+      <selection activeCell="D2" sqref="D2 D2 D2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3">
+        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
+        <v>2.0550000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
         <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2">
-        <f>VALUE(Table9[[#This Row],[Column3]])*Table9[[#This Row],[Column6]]</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f>SUM(F2:F5)</f>
-        <v>0</v>
+        <v>275.15500000000003</v>
       </c>
     </row>
   </sheetData>
@@ -770,96 +961,114 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EE7A7E-2160-4409-A677-51D38C07218F}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E9"/>
+      <selection activeCell="D2" sqref="D2 D2 D2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3">
+        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
+        <v>524.94999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
         <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
-        <f>VALUE(Table10[[#This Row],[Column3]])*Table10[[#This Row],[Column6]]</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <f>SUM(F2:F5)</f>
-        <v>0</v>
+        <v>524.94999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>